<commit_message>
Added another class with methods to print the regions, sorted by continent. Then added unittests and integration tests
</commit_message>
<xml_diff>
--- a/Assessment Tasks/Tasks for Code Reviews.xlsx
+++ b/Assessment Tasks/Tasks for Code Reviews.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Edinburgh\Software Engineering Methods\Projects\semAssessment\Assessment Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE7102F-E597-429C-966B-B197B5CF3E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2047CDC1-FB4A-4E91-AFEF-69EDA949DF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Matric</t>
   </si>
@@ -103,13 +103,19 @@
   </si>
   <si>
     <t>Program now prints list of capitals of a region</t>
+  </si>
+  <si>
+    <t>Suitable integration tests defined</t>
+  </si>
+  <si>
+    <t>Tests running on GitHub Actions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +130,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -314,6 +326,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -323,24 +348,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1006,10 +1017,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1063,7 @@
       <c r="D2" s="10">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="23">
         <v>45575</v>
       </c>
     </row>
@@ -1063,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="15"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1072,7 +1083,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="15"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
@@ -1087,7 +1098,7 @@
       <c r="D5" s="13">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -1096,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
@@ -1105,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="15"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
@@ -1114,7 +1125,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1126,10 +1137,10 @@
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="10">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -1137,8 +1148,8 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -1146,8 +1157,8 @@
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1176,10 +1187,10 @@
       <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="18">
         <v>0.25</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="22">
         <v>45596</v>
       </c>
     </row>
@@ -1189,8 +1200,7 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="28"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
@@ -1199,7 +1209,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="28"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
@@ -1211,10 +1221,10 @@
       <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="19">
         <v>0.25</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -1222,8 +1232,7 @@
       <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="28"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -1235,25 +1244,68 @@
       <c r="C21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="18">
         <v>0.25</v>
       </c>
-      <c r="E21" s="28"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
+      <c r="A22" s="14">
         <v>40690922</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="17">
         <v>0.25</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>40726424</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="29">
+        <v>45617</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Task excel updated for code review 4
</commit_message>
<xml_diff>
--- a/Assessment Tasks/Tasks for Code Reviews.xlsx
+++ b/Assessment Tasks/Tasks for Code Reviews.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Edinburgh\Software Engineering Methods\Projects\semAssessment\Assessment Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Edinburgh\Software Engineering Methods\Projects\SEMGroupRep\Assessment Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2047CDC1-FB4A-4E91-AFEF-69EDA949DF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD598A06-BEF1-4B5C-87FE-7F9127565B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Matric</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Tests running on GitHub Actions</t>
+  </si>
+  <si>
+    <t>Bug reporting system set up</t>
+  </si>
+  <si>
+    <t>Deployment working</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -307,11 +313,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -339,6 +358,10 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -348,10 +371,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1017,10 +1040,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,7 +1086,7 @@
       <c r="D2" s="10">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="27">
         <v>45575</v>
       </c>
     </row>
@@ -1074,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="24"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1083,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="24"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
@@ -1098,7 +1121,7 @@
       <c r="D5" s="13">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -1107,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="24"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
@@ -1116,7 +1139,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
@@ -1125,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1140,7 +1163,7 @@
       <c r="D9" s="10">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -1149,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="24"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -1158,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="12"/>
-      <c r="E11" s="25"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1288,24 +1311,73 @@
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="24">
         <v>1</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="26">
         <v>45617</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="21"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A33" s="14">
+        <v>40726424</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="26">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A34" s="14">
+        <v>40646484</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E34" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>